<commit_message>
Updated materials from W4-W9
Added ontrack tasks
</commit_message>
<xml_diff>
--- a/ontrack/worklog.xlsx
+++ b/ontrack/worklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuyoscar/Documents/Project/SIT723 - Research Project A/ontrack/4.1P-resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuyoscar/Documents/Project/SIT723 - Research Project A/ontrack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1457BFB0-5848-F349-93A4-88D25D1CAA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717FF3A5-2587-1046-AC29-E024C0C9CE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="2160" windowWidth="51200" windowHeight="26900" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
+    <workbookView xWindow="3800" yWindow="5000" windowWidth="38400" windowHeight="19700" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="100">
   <si>
     <t>Student Name</t>
   </si>
@@ -315,6 +315,27 @@
   </si>
   <si>
     <t>week 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>26/112021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Academic writing literature review </t>
+  </si>
+  <si>
+    <t>Academic writing method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">week 7 </t>
+  </si>
+  <si>
+    <t>week 6</t>
+  </si>
+  <si>
+    <t>review related work</t>
+  </si>
+  <si>
+    <t>week8</t>
   </si>
 </sst>
 </file>
@@ -322,7 +343,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -410,7 +431,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,17 +751,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
@@ -1095,7 +1116,7 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1114,11 +1135,15 @@
       <c r="G17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f>SUM(E3:E297)/60</f>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1142,7 +1167,7 @@
       </c>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1166,7 +1191,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1190,7 +1215,7 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1214,7 +1239,7 @@
       </c>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1238,7 +1263,7 @@
       </c>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1264,7 +1289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1288,7 +1313,7 @@
       </c>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1312,7 +1337,7 @@
       </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1336,7 +1361,7 @@
       </c>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1370,8 +1395,8 @@
       <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="7">
-        <v>44403</v>
+      <c r="D39" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="E39">
         <v>60</v>
@@ -1395,7 +1420,7 @@
         <v>41</v>
       </c>
       <c r="D40" s="7">
-        <v>44404</v>
+        <v>44527</v>
       </c>
       <c r="E40">
         <v>120</v>
@@ -1419,7 +1444,7 @@
         <v>41</v>
       </c>
       <c r="D41" s="7">
-        <v>44404</v>
+        <v>44527</v>
       </c>
       <c r="E41">
         <v>120</v>
@@ -1443,7 +1468,7 @@
         <v>41</v>
       </c>
       <c r="D42" s="7">
-        <v>44404</v>
+        <v>44527</v>
       </c>
       <c r="E42">
         <v>120</v>
@@ -1467,7 +1492,7 @@
         <v>41</v>
       </c>
       <c r="D43" s="7">
-        <v>44404</v>
+        <v>44527</v>
       </c>
       <c r="E43">
         <v>120</v>
@@ -1491,7 +1516,7 @@
         <v>41</v>
       </c>
       <c r="D44" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E44">
         <v>120</v>
@@ -1515,7 +1540,7 @@
         <v>41</v>
       </c>
       <c r="D45" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E45">
         <v>120</v>
@@ -1541,7 +1566,7 @@
         <v>41</v>
       </c>
       <c r="D46" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E46">
         <v>120</v>
@@ -1565,7 +1590,7 @@
         <v>41</v>
       </c>
       <c r="D47" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E47">
         <v>120</v>
@@ -1589,7 +1614,7 @@
         <v>41</v>
       </c>
       <c r="D48" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E48">
         <v>120</v>
@@ -1613,7 +1638,7 @@
         <v>41</v>
       </c>
       <c r="D49" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E49">
         <v>120</v>
@@ -1637,7 +1662,7 @@
         <v>41</v>
       </c>
       <c r="D50" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E50">
         <v>120</v>
@@ -1661,7 +1686,7 @@
         <v>41</v>
       </c>
       <c r="D51" s="7">
-        <v>44405</v>
+        <v>44528</v>
       </c>
       <c r="E51">
         <v>120</v>
@@ -1697,7 +1722,7 @@
         <v>41</v>
       </c>
       <c r="D56" s="7">
-        <v>44357</v>
+        <v>44510</v>
       </c>
       <c r="E56">
         <v>120</v>
@@ -1721,7 +1746,7 @@
         <v>41</v>
       </c>
       <c r="D57" s="7">
-        <v>44357</v>
+        <v>44510</v>
       </c>
       <c r="E57">
         <v>120</v>
@@ -1745,7 +1770,7 @@
         <v>41</v>
       </c>
       <c r="D58" s="7">
-        <v>44359</v>
+        <v>44512</v>
       </c>
       <c r="E58">
         <v>120</v>
@@ -1769,7 +1794,7 @@
         <v>41</v>
       </c>
       <c r="D59" s="7">
-        <v>44389</v>
+        <v>44512</v>
       </c>
       <c r="E59">
         <v>120</v>
@@ -1793,7 +1818,7 @@
         <v>41</v>
       </c>
       <c r="D60" s="7">
-        <v>44390</v>
+        <v>44513</v>
       </c>
       <c r="E60">
         <v>100</v>
@@ -1817,7 +1842,7 @@
         <v>41</v>
       </c>
       <c r="D61" s="7">
-        <v>44393</v>
+        <v>44516</v>
       </c>
       <c r="E61">
         <v>90</v>
@@ -1841,7 +1866,7 @@
         <v>41</v>
       </c>
       <c r="D62" s="7">
-        <v>44394</v>
+        <v>44517</v>
       </c>
       <c r="E62">
         <v>70</v>
@@ -1865,7 +1890,7 @@
         <v>41</v>
       </c>
       <c r="D63" s="7">
-        <v>44396</v>
+        <v>44519</v>
       </c>
       <c r="E63">
         <v>120</v>
@@ -1889,7 +1914,7 @@
         <v>41</v>
       </c>
       <c r="D64" s="7">
-        <v>44396</v>
+        <v>44519</v>
       </c>
       <c r="E64">
         <v>120</v>
@@ -1913,7 +1938,7 @@
         <v>41</v>
       </c>
       <c r="D65" s="7">
-        <v>44397</v>
+        <v>44520</v>
       </c>
       <c r="E65">
         <v>120</v>
@@ -1937,7 +1962,7 @@
         <v>41</v>
       </c>
       <c r="D66" s="7">
-        <v>44397</v>
+        <v>44520</v>
       </c>
       <c r="E66">
         <v>120</v>
@@ -1961,7 +1986,7 @@
         <v>41</v>
       </c>
       <c r="D67" s="7">
-        <v>44397</v>
+        <v>44520</v>
       </c>
       <c r="E67">
         <v>120</v>
@@ -1985,7 +2010,7 @@
         <v>41</v>
       </c>
       <c r="D68" s="7">
-        <v>44397</v>
+        <v>44520</v>
       </c>
       <c r="E68">
         <v>120</v>
@@ -2009,7 +2034,7 @@
         <v>41</v>
       </c>
       <c r="D69" s="7">
-        <v>44398</v>
+        <v>44521</v>
       </c>
       <c r="E69">
         <v>120</v>
@@ -2033,7 +2058,7 @@
         <v>41</v>
       </c>
       <c r="D70" s="7">
-        <v>44398</v>
+        <v>44521</v>
       </c>
       <c r="E70">
         <v>120</v>
@@ -2059,7 +2084,7 @@
         <v>41</v>
       </c>
       <c r="D71" s="7">
-        <v>44398</v>
+        <v>44521</v>
       </c>
       <c r="E71">
         <v>120</v>
@@ -2083,7 +2108,7 @@
         <v>41</v>
       </c>
       <c r="D72" s="7">
-        <v>44398</v>
+        <v>44521</v>
       </c>
       <c r="E72">
         <v>120</v>
@@ -2107,7 +2132,7 @@
         <v>41</v>
       </c>
       <c r="D73" s="7">
-        <v>44398</v>
+        <v>44521</v>
       </c>
       <c r="E73">
         <v>120</v>
@@ -2131,7 +2156,7 @@
         <v>41</v>
       </c>
       <c r="D74" s="7">
-        <v>44397</v>
+        <v>44524</v>
       </c>
       <c r="E74">
         <v>120</v>
@@ -2155,7 +2180,7 @@
         <v>41</v>
       </c>
       <c r="D75" s="7">
-        <v>44397</v>
+        <v>44524</v>
       </c>
       <c r="E75">
         <v>120</v>
@@ -2179,7 +2204,7 @@
         <v>41</v>
       </c>
       <c r="D76" s="7">
-        <v>44397</v>
+        <v>44524</v>
       </c>
       <c r="E76">
         <v>120</v>
@@ -2203,7 +2228,7 @@
         <v>41</v>
       </c>
       <c r="D77" s="7">
-        <v>44397</v>
+        <v>44524</v>
       </c>
       <c r="E77">
         <v>120</v>
@@ -2227,7 +2252,7 @@
         <v>41</v>
       </c>
       <c r="D78" s="7">
-        <v>44397</v>
+        <v>44524</v>
       </c>
       <c r="E78">
         <v>120</v>
@@ -2239,6 +2264,882 @@
         <v>91</v>
       </c>
       <c r="I78" s="5"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" s="7">
+        <v>44199</v>
+      </c>
+      <c r="E84">
+        <v>120</v>
+      </c>
+      <c r="F84" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" t="s">
+        <v>94</v>
+      </c>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="7">
+        <v>44199</v>
+      </c>
+      <c r="E85">
+        <v>120</v>
+      </c>
+      <c r="F85" t="s">
+        <v>13</v>
+      </c>
+      <c r="G85" t="s">
+        <v>94</v>
+      </c>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" t="s">
+        <v>41</v>
+      </c>
+      <c r="D86" s="7">
+        <v>44200</v>
+      </c>
+      <c r="E86">
+        <v>120</v>
+      </c>
+      <c r="F86" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" t="s">
+        <v>94</v>
+      </c>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="7">
+        <v>44200</v>
+      </c>
+      <c r="E87">
+        <v>120</v>
+      </c>
+      <c r="F87" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" t="s">
+        <v>94</v>
+      </c>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" t="s">
+        <v>41</v>
+      </c>
+      <c r="D88" s="7">
+        <v>44200</v>
+      </c>
+      <c r="E88">
+        <v>120</v>
+      </c>
+      <c r="F88" t="s">
+        <v>13</v>
+      </c>
+      <c r="G88" t="s">
+        <v>94</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>68</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" t="s">
+        <v>41</v>
+      </c>
+      <c r="D89" s="7">
+        <v>44201</v>
+      </c>
+      <c r="E89">
+        <v>120</v>
+      </c>
+      <c r="F89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" t="s">
+        <v>95</v>
+      </c>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>68</v>
+      </c>
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" t="s">
+        <v>41</v>
+      </c>
+      <c r="D90" s="7">
+        <v>44201</v>
+      </c>
+      <c r="E90">
+        <v>120</v>
+      </c>
+      <c r="F90" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" t="s">
+        <v>95</v>
+      </c>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" t="s">
+        <v>41</v>
+      </c>
+      <c r="D91" s="7">
+        <v>44201</v>
+      </c>
+      <c r="E91">
+        <v>120</v>
+      </c>
+      <c r="F91" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" t="s">
+        <v>94</v>
+      </c>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
+        <v>41</v>
+      </c>
+      <c r="D92" s="7">
+        <v>44202</v>
+      </c>
+      <c r="E92">
+        <v>120</v>
+      </c>
+      <c r="F92" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" t="s">
+        <v>95</v>
+      </c>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" t="s">
+        <v>41</v>
+      </c>
+      <c r="D93" s="7">
+        <v>44202</v>
+      </c>
+      <c r="E93">
+        <v>120</v>
+      </c>
+      <c r="F93" t="s">
+        <v>13</v>
+      </c>
+      <c r="G93" t="s">
+        <v>95</v>
+      </c>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>68</v>
+      </c>
+      <c r="B94" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" t="s">
+        <v>41</v>
+      </c>
+      <c r="D94" s="7">
+        <v>44202</v>
+      </c>
+      <c r="E94">
+        <v>120</v>
+      </c>
+      <c r="F94" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" t="s">
+        <v>95</v>
+      </c>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>68</v>
+      </c>
+      <c r="B99" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99" t="s">
+        <v>41</v>
+      </c>
+      <c r="D99" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E99">
+        <v>120</v>
+      </c>
+      <c r="F99" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" t="s">
+        <v>94</v>
+      </c>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>68</v>
+      </c>
+      <c r="B100" t="s">
+        <v>24</v>
+      </c>
+      <c r="C100" t="s">
+        <v>41</v>
+      </c>
+      <c r="D100" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E100">
+        <v>120</v>
+      </c>
+      <c r="F100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" t="s">
+        <v>94</v>
+      </c>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>68</v>
+      </c>
+      <c r="B101" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" t="s">
+        <v>41</v>
+      </c>
+      <c r="D101" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E101">
+        <v>120</v>
+      </c>
+      <c r="F101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" t="s">
+        <v>94</v>
+      </c>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>68</v>
+      </c>
+      <c r="B102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" t="s">
+        <v>41</v>
+      </c>
+      <c r="D102" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E102">
+        <v>120</v>
+      </c>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102" t="s">
+        <v>94</v>
+      </c>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>68</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>41</v>
+      </c>
+      <c r="D103" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E103">
+        <v>120</v>
+      </c>
+      <c r="F103" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" t="s">
+        <v>94</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>68</v>
+      </c>
+      <c r="B104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" t="s">
+        <v>41</v>
+      </c>
+      <c r="D104" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E104">
+        <v>120</v>
+      </c>
+      <c r="F104" t="s">
+        <v>13</v>
+      </c>
+      <c r="G104" t="s">
+        <v>95</v>
+      </c>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B105" t="s">
+        <v>24</v>
+      </c>
+      <c r="C105" t="s">
+        <v>41</v>
+      </c>
+      <c r="D105" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E105">
+        <v>120</v>
+      </c>
+      <c r="F105" t="s">
+        <v>13</v>
+      </c>
+      <c r="G105" t="s">
+        <v>95</v>
+      </c>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106" t="s">
+        <v>24</v>
+      </c>
+      <c r="C106" t="s">
+        <v>41</v>
+      </c>
+      <c r="D106" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E106">
+        <v>120</v>
+      </c>
+      <c r="F106" t="s">
+        <v>13</v>
+      </c>
+      <c r="G106" t="s">
+        <v>94</v>
+      </c>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107" t="s">
+        <v>24</v>
+      </c>
+      <c r="C107" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E107">
+        <v>120</v>
+      </c>
+      <c r="F107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G107" t="s">
+        <v>95</v>
+      </c>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>68</v>
+      </c>
+      <c r="B108" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108" t="s">
+        <v>41</v>
+      </c>
+      <c r="D108" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E108">
+        <v>120</v>
+      </c>
+      <c r="F108" t="s">
+        <v>13</v>
+      </c>
+      <c r="G108" t="s">
+        <v>95</v>
+      </c>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>68</v>
+      </c>
+      <c r="B109" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" t="s">
+        <v>41</v>
+      </c>
+      <c r="D109" s="7">
+        <v>44553</v>
+      </c>
+      <c r="E109">
+        <v>120</v>
+      </c>
+      <c r="F109" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" t="s">
+        <v>95</v>
+      </c>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D110" s="7"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>68</v>
+      </c>
+      <c r="B113" t="s">
+        <v>24</v>
+      </c>
+      <c r="C113" t="s">
+        <v>41</v>
+      </c>
+      <c r="D113" s="7">
+        <v>44205</v>
+      </c>
+      <c r="E113">
+        <v>120</v>
+      </c>
+      <c r="F113" t="s">
+        <v>13</v>
+      </c>
+      <c r="G113" t="s">
+        <v>98</v>
+      </c>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>68</v>
+      </c>
+      <c r="B114" t="s">
+        <v>24</v>
+      </c>
+      <c r="C114" t="s">
+        <v>41</v>
+      </c>
+      <c r="D114" s="7">
+        <v>44207</v>
+      </c>
+      <c r="E114">
+        <v>120</v>
+      </c>
+      <c r="F114" t="s">
+        <v>13</v>
+      </c>
+      <c r="G114" t="s">
+        <v>98</v>
+      </c>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>68</v>
+      </c>
+      <c r="B115" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" t="s">
+        <v>41</v>
+      </c>
+      <c r="D115" s="7">
+        <v>44207</v>
+      </c>
+      <c r="E115">
+        <v>120</v>
+      </c>
+      <c r="F115" t="s">
+        <v>13</v>
+      </c>
+      <c r="G115" t="s">
+        <v>95</v>
+      </c>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>68</v>
+      </c>
+      <c r="B116" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" t="s">
+        <v>41</v>
+      </c>
+      <c r="D116" s="7">
+        <v>44207</v>
+      </c>
+      <c r="E116">
+        <v>120</v>
+      </c>
+      <c r="F116" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" t="s">
+        <v>95</v>
+      </c>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>68</v>
+      </c>
+      <c r="B117" t="s">
+        <v>24</v>
+      </c>
+      <c r="C117" t="s">
+        <v>41</v>
+      </c>
+      <c r="D117" s="7">
+        <v>44207</v>
+      </c>
+      <c r="E117">
+        <v>120</v>
+      </c>
+      <c r="F117" t="s">
+        <v>13</v>
+      </c>
+      <c r="G117" t="s">
+        <v>95</v>
+      </c>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>68</v>
+      </c>
+      <c r="B118" t="s">
+        <v>24</v>
+      </c>
+      <c r="C118" t="s">
+        <v>41</v>
+      </c>
+      <c r="D118" s="7">
+        <v>44208</v>
+      </c>
+      <c r="E118">
+        <v>120</v>
+      </c>
+      <c r="F118" t="s">
+        <v>13</v>
+      </c>
+      <c r="G118" t="s">
+        <v>95</v>
+      </c>
+      <c r="I118" s="5"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>68</v>
+      </c>
+      <c r="B119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C119" t="s">
+        <v>41</v>
+      </c>
+      <c r="D119" s="7">
+        <v>44208</v>
+      </c>
+      <c r="E119">
+        <v>120</v>
+      </c>
+      <c r="F119" t="s">
+        <v>13</v>
+      </c>
+      <c r="G119" t="s">
+        <v>95</v>
+      </c>
+      <c r="I119" s="5"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>68</v>
+      </c>
+      <c r="B120" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" t="s">
+        <v>41</v>
+      </c>
+      <c r="D120" s="7">
+        <v>44208</v>
+      </c>
+      <c r="E120">
+        <v>120</v>
+      </c>
+      <c r="F120" t="s">
+        <v>13</v>
+      </c>
+      <c r="G120" t="s">
+        <v>95</v>
+      </c>
+      <c r="I120" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>68</v>
+      </c>
+      <c r="B121" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121" t="s">
+        <v>41</v>
+      </c>
+      <c r="D121" s="7">
+        <v>44209</v>
+      </c>
+      <c r="E121">
+        <v>120</v>
+      </c>
+      <c r="F121" t="s">
+        <v>13</v>
+      </c>
+      <c r="G121" t="s">
+        <v>95</v>
+      </c>
+      <c r="I121" s="5"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>68</v>
+      </c>
+      <c r="B122" t="s">
+        <v>24</v>
+      </c>
+      <c r="C122" t="s">
+        <v>41</v>
+      </c>
+      <c r="D122" s="7">
+        <v>44209</v>
+      </c>
+      <c r="E122">
+        <v>120</v>
+      </c>
+      <c r="F122" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" t="s">
+        <v>95</v>
+      </c>
+      <c r="I122" s="5"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>68</v>
+      </c>
+      <c r="B123" t="s">
+        <v>24</v>
+      </c>
+      <c r="C123" t="s">
+        <v>41</v>
+      </c>
+      <c r="D123" s="7">
+        <v>44209</v>
+      </c>
+      <c r="E123">
+        <v>120</v>
+      </c>
+      <c r="F123" t="s">
+        <v>13</v>
+      </c>
+      <c r="G123" t="s">
+        <v>95</v>
+      </c>
+      <c r="I123" s="5"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>68</v>
+      </c>
+      <c r="B124" t="s">
+        <v>24</v>
+      </c>
+      <c r="C124" t="s">
+        <v>41</v>
+      </c>
+      <c r="D124" s="7">
+        <v>44210</v>
+      </c>
+      <c r="E124">
+        <v>120</v>
+      </c>
+      <c r="F124" t="s">
+        <v>13</v>
+      </c>
+      <c r="G124" t="s">
+        <v>95</v>
+      </c>
+      <c r="I124" s="5"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>68</v>
+      </c>
+      <c r="B125" t="s">
+        <v>24</v>
+      </c>
+      <c r="C125" t="s">
+        <v>41</v>
+      </c>
+      <c r="D125" s="7">
+        <v>44211</v>
+      </c>
+      <c r="E125">
+        <v>120</v>
+      </c>
+      <c r="F125" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125" t="s">
+        <v>95</v>
+      </c>
+      <c r="I125" s="5"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>68</v>
+      </c>
+      <c r="B126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C126" t="s">
+        <v>41</v>
+      </c>
+      <c r="D126" s="7">
+        <v>44212</v>
+      </c>
+      <c r="E126">
+        <v>120</v>
+      </c>
+      <c r="F126" t="s">
+        <v>13</v>
+      </c>
+      <c r="G126" t="s">
+        <v>95</v>
+      </c>
+      <c r="I126" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2378,6 +3279,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2386,7 +3293,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F91A6F9DB61C7A45BED08E943CE76CDB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e8e7f53c33be68033672446c1e6efa23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01b46ff2-420f-42c8-8583-78d94109e361" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfdeac3786ae83719fa373dd0d32d08c" ns2:_="">
     <xsd:import namespace="01b46ff2-420f-42c8-8583-78d94109e361"/>
@@ -2518,13 +3425,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2532,7 +3442,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FB1FFC3-B1E9-4426-A852-9D9BC12D3CD6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2548,13 +3458,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>